<commit_message>
Leitura de Titulo e Abstract
Terminado
</commit_message>
<xml_diff>
--- a/artigos_ACM/SelecaoFase1_Lidia.xlsx
+++ b/artigos_ACM/SelecaoFase1_Lidia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Mestrado\slr\artigos_ACM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Mestrado2\slr\artigos_ACM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9AFDE8-F5FC-4CEA-BEDE-6318D84DF2FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893D9854-9FA6-43B7-8DCA-8BD89A931D39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1A65388C-AACB-4B7E-B60C-47E18581C927}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="161">
   <si>
     <t>type</t>
   </si>
@@ -1019,20 +1019,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7271E0F0-47A0-43BD-A095-D2B08052F9FE}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" customWidth="1"/>
-    <col min="4" max="4" width="81.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="7.140625" customWidth="1"/>
-    <col min="6" max="6" width="4" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
@@ -1158,6 +1158,12 @@
       <c r="E5">
         <v>2008</v>
       </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>150</v>
+      </c>
       <c r="H5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1233,6 +1239,9 @@
       <c r="E8">
         <v>2012</v>
       </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
       <c r="G8" t="s">
         <v>150</v>
       </c>
@@ -1256,6 +1265,12 @@
       <c r="E9">
         <v>2011</v>
       </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>150</v>
+      </c>
       <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1305,6 +1320,12 @@
       <c r="E11">
         <v>2011</v>
       </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>150</v>
+      </c>
       <c r="H11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1415,6 +1436,9 @@
       <c r="E16">
         <v>2011</v>
       </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
       <c r="G16" t="s">
         <v>150</v>
       </c>
@@ -1438,6 +1462,9 @@
       <c r="E17">
         <v>2007</v>
       </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
       <c r="H17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1518,6 +1545,12 @@
       <c r="E21">
         <v>2005</v>
       </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>150</v>
+      </c>
       <c r="H21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1561,6 +1594,12 @@
       <c r="E23">
         <v>2010</v>
       </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>150</v>
+      </c>
       <c r="H23" s="1" t="s">
         <v>74</v>
       </c>
@@ -1661,6 +1700,12 @@
       <c r="E28">
         <v>2014</v>
       </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>150</v>
+      </c>
       <c r="H28" s="1" t="s">
         <v>11</v>
       </c>
@@ -1701,6 +1746,12 @@
       <c r="E30">
         <v>2013</v>
       </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>150</v>
+      </c>
       <c r="H30" s="1" t="s">
         <v>11</v>
       </c>
@@ -1767,6 +1818,12 @@
       <c r="E33">
         <v>2012</v>
       </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33" t="s">
+        <v>150</v>
+      </c>
       <c r="H33" s="1" t="s">
         <v>11</v>
       </c>
@@ -1859,6 +1916,12 @@
       <c r="E37">
         <v>2012</v>
       </c>
+      <c r="F37">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>150</v>
+      </c>
       <c r="H37" s="1" t="s">
         <v>11</v>
       </c>
@@ -1879,6 +1942,12 @@
       <c r="E38">
         <v>2014</v>
       </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>150</v>
+      </c>
       <c r="H38" s="1" t="s">
         <v>11</v>
       </c>
@@ -1899,6 +1968,12 @@
       <c r="E39">
         <v>2011</v>
       </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39" t="s">
+        <v>150</v>
+      </c>
       <c r="H39" s="1" t="s">
         <v>11</v>
       </c>
@@ -1982,6 +2057,12 @@
       <c r="E43">
         <v>2012</v>
       </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43" t="s">
+        <v>150</v>
+      </c>
       <c r="H43" s="1" t="s">
         <v>11</v>
       </c>
@@ -2002,6 +2083,12 @@
       <c r="E44">
         <v>2014</v>
       </c>
+      <c r="F44">
+        <v>5</v>
+      </c>
+      <c r="G44" t="s">
+        <v>150</v>
+      </c>
       <c r="H44" s="1" t="s">
         <v>135</v>
       </c>
@@ -2022,6 +2109,12 @@
       <c r="E45">
         <v>2012</v>
       </c>
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="G45" t="s">
+        <v>150</v>
+      </c>
       <c r="H45" s="1" t="s">
         <v>11</v>
       </c>
@@ -2042,6 +2135,9 @@
       <c r="E46">
         <v>2010</v>
       </c>
+      <c r="F46">
+        <v>5</v>
+      </c>
       <c r="G46" t="s">
         <v>150</v>
       </c>
@@ -2064,6 +2160,12 @@
       </c>
       <c r="E47">
         <v>2011</v>
+      </c>
+      <c r="F47">
+        <v>5</v>
+      </c>
+      <c r="G47" t="s">
+        <v>150</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>11</v>

</xml_diff>